<commit_message>
nb: add comments about trial label
</commit_message>
<xml_diff>
--- a/results/2024_02_13_rce2_spike_analysis/data/rce_per_subject_start_stop_video_frame.xlsx
+++ b/results/2024_02_13_rce2_spike_analysis/data/rce_per_subject_start_stop_video_frame.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27417"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="352" documentId="11_62D7479E5772F09A29C9EFE5FCBFF434EA66B218" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A136424-FF4F-4BA9-B9D9-9FDD2A542D20}"/>
+  <xr:revisionPtr revIDLastSave="404" documentId="11_62D7479E5772F09A29C9EFE5FCBFF434EA66B218" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67EF23DF-25C1-41D8-97B9-99400E68F45B}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="63">
   <si>
     <t>file_path</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>in_video_subjects</t>
+  </si>
+  <si>
+    <t>box_number</t>
   </si>
   <si>
     <t>notes</t>
@@ -271,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -283,15 +286,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -608,11 +602,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
+      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -620,12 +614,12 @@
     <col min="1" max="1" width="102.42578125" style="1" customWidth="1"/>
     <col min="2" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="15.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="50.140625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="50.140625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30.75">
+    <row r="1" spans="1:7" ht="30.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -644,10 +638,13 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -659,12 +656,15 @@
         <v>6.3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1">
         <v>27500</v>
@@ -673,15 +673,18 @@
         <v>73600</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1">
         <v>51500</v>
@@ -693,12 +696,15 @@
         <v>6.3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -707,253 +713,295 @@
         <v>48500</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="6" customFormat="1">
-      <c r="A6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="5">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2">
         <v>32700</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="2">
         <v>68257</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="2">
         <v>1.2</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" s="6" customFormat="1">
-      <c r="A7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="5">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="E6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
         <v>32300</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" s="6" customFormat="1">
-      <c r="A8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="5">
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2">
         <v>33000</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="2">
         <v>68212</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" s="6" customFormat="1">
-      <c r="A9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="5">
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="2">
+        <v>2</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2">
         <v>33400</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="2">
         <v>68332</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" s="6" customFormat="1">
-      <c r="A10" s="5" t="s">
+      <c r="E9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="5">
-        <v>1</v>
-      </c>
-      <c r="C10" s="5">
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
         <v>33000</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" s="7" customFormat="1">
-      <c r="A11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="5">
+      <c r="D10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" s="3" customFormat="1">
+      <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2">
         <v>33700</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="2">
         <v>68292</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="2">
         <v>1.4</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" s="7" customFormat="1">
-      <c r="A12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="5">
+      <c r="E11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="2">
+        <v>2</v>
+      </c>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" s="3" customFormat="1">
+      <c r="A12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2">
         <v>32800</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="2">
         <v>44205</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" s="7" customFormat="1">
-      <c r="A13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="5">
-        <v>1</v>
-      </c>
-      <c r="C13" s="5">
+      <c r="E12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" s="3" customFormat="1">
+      <c r="A13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
         <v>32200</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" s="7" customFormat="1">
-      <c r="A14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="5">
+      <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" s="3" customFormat="1">
+      <c r="A14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="2">
         <v>41600</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="2">
         <v>75829</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="2">
         <v>1.2</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="7" customFormat="1">
-      <c r="A15" s="5" t="s">
+      <c r="E14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="5">
-        <v>1</v>
-      </c>
-      <c r="C15" s="5">
+    </row>
+    <row r="15" spans="1:7" s="3" customFormat="1">
+      <c r="A15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
         <v>23574</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" s="7" customFormat="1">
-      <c r="A16" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="5">
+      <c r="E15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" s="3" customFormat="1">
+      <c r="A16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="2">
         <v>32100</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="2">
         <v>67369</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="2">
         <v>1.4</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:6" s="7" customFormat="1">
-      <c r="A17" s="5" t="s">
+      <c r="E16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="5">
-        <v>1</v>
-      </c>
-      <c r="C17" s="5">
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" s="3" customFormat="1">
+      <c r="A17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2">
         <v>31100</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="1:6" s="7" customFormat="1">
-      <c r="A18" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="5">
+      <c r="D17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" s="3" customFormat="1">
+      <c r="A18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="2">
         <v>36100</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="2">
         <v>71644</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="2">
         <v>1.2</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="3" customFormat="1">
+      <c r="E18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="3" customFormat="1">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19" s="1">
         <v>41000</v>
@@ -965,13 +1013,16 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" s="3" customFormat="1">
+        <v>13</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" s="3" customFormat="1">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
@@ -980,16 +1031,19 @@
         <v>39500</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" s="3" customFormat="1">
+        <v>13</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" s="3" customFormat="1">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
@@ -1001,13 +1055,16 @@
         <v>1.2</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" s="3" customFormat="1">
+        <v>13</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" s="3" customFormat="1">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B22" s="1">
         <v>32792</v>
@@ -1019,12 +1076,15 @@
         <v>1.4</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>17</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B23" s="1">
         <v>1</v>
@@ -1033,16 +1093,19 @@
         <v>32316</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:6">
+        <v>17</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B24" s="1">
         <v>32792</v>
@@ -1054,13 +1117,16 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6">
+        <v>17</v>
+      </c>
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B25" s="1">
         <v>32500</v>
@@ -1072,13 +1138,16 @@
         <v>1.2</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" s="4" customFormat="1">
+        <v>26</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" s="4" customFormat="1">
       <c r="A26" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
@@ -1087,16 +1156,19 @@
         <v>30000</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" s="4" customFormat="1">
+        <v>26</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" s="4" customFormat="1">
       <c r="A27" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B27" s="1">
         <v>32500</v>
@@ -1108,13 +1180,16 @@
         <v>1.4</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="1:6" s="4" customFormat="1">
+        <v>26</v>
+      </c>
+      <c r="F27" s="1">
+        <v>2</v>
+      </c>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" s="4" customFormat="1">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B28" s="1">
         <v>32860</v>
@@ -1126,13 +1201,16 @@
         <v>1.2</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" s="4" customFormat="1">
+        <v>13</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="3"/>
+    </row>
+    <row r="29" spans="1:7" s="4" customFormat="1">
       <c r="A29" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B29" s="1">
         <v>2027</v>
@@ -1141,16 +1219,19 @@
         <v>32239</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="1:6" s="4" customFormat="1">
+        <v>13</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="1:7" s="4" customFormat="1">
       <c r="A30" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B30" s="1">
         <v>32860</v>
@@ -1162,13 +1243,16 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="1:6" s="4" customFormat="1">
+        <v>13</v>
+      </c>
+      <c r="F30" s="1">
+        <v>2</v>
+      </c>
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="1:7" s="4" customFormat="1">
       <c r="A31" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B31" s="2">
         <v>35000</v>
@@ -1180,13 +1264,16 @@
         <v>1.4</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:6" s="4" customFormat="1">
+        <v>26</v>
+      </c>
+      <c r="F31" s="2">
+        <v>1</v>
+      </c>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" s="4" customFormat="1">
       <c r="A32" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B32" s="2">
         <v>1</v>
@@ -1195,16 +1282,19 @@
         <v>33500</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:6" s="4" customFormat="1">
+        <v>26</v>
+      </c>
+      <c r="F32" s="2">
+        <v>1</v>
+      </c>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" s="4" customFormat="1">
       <c r="A33" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B33" s="2">
         <v>34500</v>
@@ -1216,13 +1306,16 @@
         <v>1.2</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="1:6" s="4" customFormat="1">
+        <v>26</v>
+      </c>
+      <c r="F33" s="2">
+        <v>2</v>
+      </c>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" s="4" customFormat="1">
       <c r="A34" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B34" s="1">
         <v>1</v>
@@ -1231,16 +1324,19 @@
         <v>73111</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="1:6" s="4" customFormat="1">
+        <v>13</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1</v>
+      </c>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" s="4" customFormat="1">
       <c r="A35" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B35" s="1">
         <v>1</v>
@@ -1249,16 +1345,19 @@
         <v>11733</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="1:6" s="4" customFormat="1">
+        <v>17</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1</v>
+      </c>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" s="4" customFormat="1">
       <c r="A36" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B36" s="1">
         <v>1</v>
@@ -1267,16 +1366,19 @@
         <v>60699</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="1:6" s="4" customFormat="1">
+        <v>17</v>
+      </c>
+      <c r="F36" s="1">
+        <v>1</v>
+      </c>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" s="4" customFormat="1">
       <c r="A37" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B37" s="1">
         <v>1</v>
@@ -1285,16 +1387,19 @@
         <v>72635</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="1:6" s="4" customFormat="1">
+        <v>26</v>
+      </c>
+      <c r="F37" s="1">
+        <v>1</v>
+      </c>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" s="4" customFormat="1">
       <c r="A38" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B38" s="1">
         <v>1</v>
@@ -1303,16 +1408,19 @@
         <v>73292</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F38" s="1"/>
-    </row>
-    <row r="39" spans="1:6">
+        <v>17</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1</v>
+      </c>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B39" s="1">
         <v>1</v>
@@ -1321,15 +1429,18 @@
         <v>31500</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>13</v>
+      </c>
+      <c r="F39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B40" s="1">
         <v>37500</v>
@@ -1338,15 +1449,18 @@
         <v>69199</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>50</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B41" s="1">
         <v>1</v>
@@ -1355,16 +1469,19 @@
         <v>1918</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F41" s="3"/>
-    </row>
-    <row r="42" spans="1:6">
+        <v>52</v>
+      </c>
+      <c r="F41" s="1">
+        <v>2</v>
+      </c>
+      <c r="G41" s="3"/>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B42" s="1">
         <v>1</v>
@@ -1373,16 +1490,19 @@
         <v>29500</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F42" s="3"/>
-    </row>
-    <row r="43" spans="1:6">
+        <v>52</v>
+      </c>
+      <c r="F42" s="1">
+        <v>2</v>
+      </c>
+      <c r="G42" s="3"/>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B43" s="1">
         <v>1</v>
@@ -1391,16 +1511,19 @@
         <v>1466</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F43" s="3"/>
-    </row>
-    <row r="44" spans="1:6">
+        <v>50</v>
+      </c>
+      <c r="F43" s="1">
+        <v>2</v>
+      </c>
+      <c r="G43" s="3"/>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B44" s="1">
         <v>1</v>
@@ -1409,15 +1532,18 @@
         <v>31500</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>17</v>
+      </c>
+      <c r="F44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B45" s="1">
         <v>38000</v>
@@ -1426,15 +1552,18 @@
         <v>69884</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>56</v>
+      </c>
+      <c r="F45" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B46" s="1">
         <v>1</v>
@@ -1443,15 +1572,18 @@
         <v>31500</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>52</v>
+      </c>
+      <c r="F46" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B47" s="1">
         <v>37500</v>
@@ -1460,15 +1592,18 @@
         <v>69803</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>58</v>
+      </c>
+      <c r="F47" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B48" s="1">
         <v>1</v>
@@ -1477,15 +1612,18 @@
         <v>32200</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+        <v>26</v>
+      </c>
+      <c r="F48" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B49" s="1">
         <v>38000</v>
@@ -1494,15 +1632,18 @@
         <v>69950</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+        <v>60</v>
+      </c>
+      <c r="F49" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B50" s="1">
         <v>1</v>
@@ -1511,15 +1652,18 @@
         <v>31000</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+        <v>52</v>
+      </c>
+      <c r="F50" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B51" s="1">
         <v>36500</v>
@@ -1528,14 +1672,17 @@
         <v>68592</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="F51" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F1048576">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G1048576">
     <sortCondition ref="A2:A1048576"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>